<commit_message>
add selection of terms
</commit_message>
<xml_diff>
--- a/classification_of_payment_documents/example_table.xlsx
+++ b/classification_of_payment_documents/example_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasialavrova/diplom/bmstu_bachelor_qualification_work/classification_of_payment_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F32C120-200B-9C4E-BED9-3E80C1B3C8DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EB64ED-226A-8C49-A2E9-7D53418DC7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="1000" windowWidth="27640" windowHeight="15100" xr2:uid="{0D99C4A0-3FAD-3F4A-9C43-A9C82BCCA544}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Получение денежных средств на р/с</t>
   </si>
   <si>
-    <t>ЗА 10/02/2020;БЫЧКОВА АНАСТАСИЯ ВЛАДИМИРОВНА;ОПЛ. УСЛУГ СТРАХОВАНИЯ ПО ДОГОВОРУ НАКОПИТЕЛЬНОГО СТРАХОВАНИЯ ЖИЗНИ №0340780408052 ОТ 15 ИЮНЯ 2018</t>
-  </si>
-  <si>
     <t>ЗА 10/02/2020;КУТЛУЮЛОВА ДИЛЯ РАФАЭЛОВНА;0340020443303</t>
   </si>
   <si>
@@ -832,6 +829,9 @@
   </si>
   <si>
     <t>ВЫПЛАТА КД ПО ОБЛИГАЦИЯМ ПАО "ГАЗПРОМ НЕФТЬ" (РАЗМЕР КУП.ДОХОДА НА 1ЦБ - 39.14РУБ.), ГРН 4B02-03-00146-A-001P , КОЛ-ВО ЦБ - 166601ШТ. БЕЗНДС</t>
+  </si>
+  <si>
+    <t>ЗА 10/02/2020;БЫЧКОВА "АНАСТАСИЯ" ВЛАДИМИРОВНА;ОПЛ. УСЛУГ СТРАХОВАНИЯ ПО ДОГОВОРУ НАКОПИТЕЛЬНОГО СТРАХОВАНИЯ ЖИЗНИ №0340780408052 ОТ 15 ИЮНЯ 2018</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0A4823-B8C1-F54A-A299-81C21B5A1A62}">
   <dimension ref="A1:H297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="G311" sqref="G311"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="H2" s="1">
         <v>2490286</v>
@@ -1289,7 +1289,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
         <v>2490286</v>
@@ -1315,7 +1315,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="1">
         <v>2469933</v>
@@ -1341,7 +1341,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1">
         <v>2469933</v>
@@ -1367,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1">
         <v>2469933</v>
@@ -1393,7 +1393,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1">
         <v>2469933</v>
@@ -1419,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="1">
         <v>2469933</v>
@@ -1445,7 +1445,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1">
         <v>2469933</v>
@@ -1471,7 +1471,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="1">
         <v>2469933</v>
@@ -1497,7 +1497,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1">
         <v>2469933</v>
@@ -1523,7 +1523,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1">
         <v>2469933</v>
@@ -1549,7 +1549,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1">
         <v>2469933</v>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1">
         <v>2469933</v>
@@ -1601,7 +1601,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1">
         <v>2469933</v>
@@ -1627,7 +1627,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1">
         <v>2469933</v>
@@ -1653,7 +1653,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="1">
         <v>2469933</v>
@@ -1679,7 +1679,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="1">
         <v>2469933</v>
@@ -1705,7 +1705,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1">
         <v>2466314</v>
@@ -1731,7 +1731,7 @@
         <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="1">
         <v>2466315</v>
@@ -1757,7 +1757,7 @@
         <v>9</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H21" s="1">
         <v>2466315</v>
@@ -1783,7 +1783,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="1">
         <v>2466315</v>
@@ -1809,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="1">
         <v>2466315</v>
@@ -1835,7 +1835,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H24" s="1">
         <v>2466315</v>
@@ -1861,7 +1861,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="1">
         <v>2467260</v>
@@ -1887,7 +1887,7 @@
         <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="1">
         <v>2467261</v>
@@ -1913,7 +1913,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" s="1">
         <v>2467261</v>
@@ -1939,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" s="1">
         <v>2467261</v>
@@ -1965,7 +1965,7 @@
         <v>9</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H29" s="1">
         <v>2467261</v>
@@ -1991,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="1">
         <v>2467261</v>
@@ -2017,7 +2017,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H31" s="1">
         <v>2467261</v>
@@ -2043,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="1">
         <v>2467261</v>
@@ -2069,7 +2069,7 @@
         <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1">
         <v>2467261</v>
@@ -2095,7 +2095,7 @@
         <v>9</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H34" s="1">
         <v>2467263</v>
@@ -2121,7 +2121,7 @@
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H35" s="1">
         <v>2469315</v>
@@ -2147,7 +2147,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="1">
         <v>2469316</v>
@@ -2173,7 +2173,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H37" s="1">
         <v>2469316</v>
@@ -2199,7 +2199,7 @@
         <v>9</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H38" s="1">
         <v>2469316</v>
@@ -2225,7 +2225,7 @@
         <v>9</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" s="1">
         <v>2469316</v>
@@ -2251,7 +2251,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H40" s="1">
         <v>2469316</v>
@@ -2277,7 +2277,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H41" s="1">
         <v>2469316</v>
@@ -2303,7 +2303,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H42" s="1">
         <v>2469316</v>
@@ -2329,7 +2329,7 @@
         <v>9</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H43" s="1">
         <v>2469316</v>
@@ -2355,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H44" s="1">
         <v>2469316</v>
@@ -2381,7 +2381,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H45" s="1">
         <v>2469316</v>
@@ -2407,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H46" s="1">
         <v>2469316</v>
@@ -2433,7 +2433,7 @@
         <v>9</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H47" s="1">
         <v>2469316</v>
@@ -2459,7 +2459,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="1">
         <v>2469316</v>
@@ -2485,7 +2485,7 @@
         <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H49" s="1">
         <v>2469316</v>
@@ -2511,7 +2511,7 @@
         <v>9</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H50" s="1">
         <v>2469316</v>
@@ -2534,10 +2534,10 @@
         <v>1801</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H51" s="1">
         <v>2466314</v>
@@ -2560,10 +2560,10 @@
         <v>1801</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H52" s="1">
         <v>2466314</v>
@@ -2586,10 +2586,10 @@
         <v>1801</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H53" s="1">
         <v>2466314</v>
@@ -2612,10 +2612,10 @@
         <v>1801</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H54" s="1">
         <v>2466314</v>
@@ -2638,10 +2638,10 @@
         <v>1801</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H55" s="1">
         <v>2466314</v>
@@ -2664,10 +2664,10 @@
         <v>1801</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H56" s="1">
         <v>2466314</v>
@@ -2690,10 +2690,10 @@
         <v>1801</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H57" s="1">
         <v>2466315</v>
@@ -2716,10 +2716,10 @@
         <v>1801</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H58" s="1">
         <v>2466315</v>
@@ -2742,10 +2742,10 @@
         <v>1801</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H59" s="1">
         <v>2466315</v>
@@ -2768,10 +2768,10 @@
         <v>1801</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H60" s="1">
         <v>2466315</v>
@@ -2794,10 +2794,10 @@
         <v>1801</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H61" s="1">
         <v>2466315</v>
@@ -2820,10 +2820,10 @@
         <v>1801</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H62" s="1">
         <v>2466315</v>
@@ -2846,10 +2846,10 @@
         <v>1801</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H63" s="1">
         <v>2466315</v>
@@ -2872,10 +2872,10 @@
         <v>1801</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H64" s="1">
         <v>2469933</v>
@@ -2898,10 +2898,10 @@
         <v>1801</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H65" s="1">
         <v>2469933</v>
@@ -2924,10 +2924,10 @@
         <v>1801</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H66" s="1">
         <v>2469933</v>
@@ -2950,10 +2950,10 @@
         <v>1801</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H67" s="1">
         <v>2467260</v>
@@ -2976,10 +2976,10 @@
         <v>1801</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H68" s="1">
         <v>2467260</v>
@@ -3002,10 +3002,10 @@
         <v>1801</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H69" s="1">
         <v>2467261</v>
@@ -3028,10 +3028,10 @@
         <v>1801</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H70" s="1">
         <v>2467261</v>
@@ -3054,10 +3054,10 @@
         <v>1801</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H71" s="1">
         <v>2467261</v>
@@ -3080,10 +3080,10 @@
         <v>1801</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H72" s="1">
         <v>2467261</v>
@@ -3106,10 +3106,10 @@
         <v>1801</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H73" s="1">
         <v>2468156</v>
@@ -3132,10 +3132,10 @@
         <v>1801</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H74" s="1">
         <v>2468156</v>
@@ -3158,10 +3158,10 @@
         <v>1801</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H75" s="1">
         <v>2469315</v>
@@ -3184,10 +3184,10 @@
         <v>1801</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H76" s="1">
         <v>2469315</v>
@@ -3210,10 +3210,10 @@
         <v>1801</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H77" s="1">
         <v>2469316</v>
@@ -3236,10 +3236,10 @@
         <v>1801</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H78" s="1">
         <v>2469316</v>
@@ -3262,10 +3262,10 @@
         <v>1801</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H79" s="1">
         <v>2469316</v>
@@ -3288,10 +3288,10 @@
         <v>1801</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H80" s="1">
         <v>2469933</v>
@@ -3314,10 +3314,10 @@
         <v>1801</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H81" s="1">
         <v>2470866</v>
@@ -3340,10 +3340,10 @@
         <v>1801</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H82" s="1">
         <v>2470867</v>
@@ -3366,10 +3366,10 @@
         <v>1801</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H83" s="1">
         <v>2470867</v>
@@ -3392,10 +3392,10 @@
         <v>1801</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H84" s="1">
         <v>2470867</v>
@@ -3418,10 +3418,10 @@
         <v>1801</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H85" s="1">
         <v>2470867</v>
@@ -3444,10 +3444,10 @@
         <v>1801</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H86" s="1">
         <v>2470867</v>
@@ -3470,10 +3470,10 @@
         <v>1801</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H87" s="1">
         <v>2470867</v>
@@ -3496,10 +3496,10 @@
         <v>1801</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H88" s="1">
         <v>2470867</v>
@@ -3522,10 +3522,10 @@
         <v>1801</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H89" s="1">
         <v>2470867</v>
@@ -3548,10 +3548,10 @@
         <v>1801</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H90" s="1">
         <v>2470867</v>
@@ -3574,10 +3574,10 @@
         <v>1801</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H91" s="1">
         <v>2470867</v>
@@ -3600,10 +3600,10 @@
         <v>1801</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H92" s="1">
         <v>2470867</v>
@@ -3626,10 +3626,10 @@
         <v>1801</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H93" s="1">
         <v>2470867</v>
@@ -3652,10 +3652,10 @@
         <v>1801</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H94" s="1">
         <v>2470868</v>
@@ -3678,10 +3678,10 @@
         <v>1801</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H95" s="1">
         <v>2471898</v>
@@ -3704,10 +3704,10 @@
         <v>1801</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H96" s="1">
         <v>2471898</v>
@@ -3730,10 +3730,10 @@
         <v>1801</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H97" s="1">
         <v>2471899</v>
@@ -3756,10 +3756,10 @@
         <v>1801</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H98" s="1">
         <v>2472782</v>
@@ -3782,10 +3782,10 @@
         <v>1801</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H99" s="1">
         <v>2480853</v>
@@ -3808,10 +3808,10 @@
         <v>1801</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H100" s="1">
         <v>2480854</v>
@@ -3834,10 +3834,10 @@
         <v>2295</v>
       </c>
       <c r="F101" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="H101" s="1">
         <v>2469315</v>
@@ -3860,10 +3860,10 @@
         <v>2295</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H102" s="1">
         <v>2470866</v>
@@ -3886,10 +3886,10 @@
         <v>2295</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H103" s="1">
         <v>2470868</v>
@@ -3912,10 +3912,10 @@
         <v>2295</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H104" s="1">
         <v>2471899</v>
@@ -3938,10 +3938,10 @@
         <v>2295</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H105" s="1">
         <v>2466314</v>
@@ -3964,10 +3964,10 @@
         <v>2295</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H106" s="1">
         <v>2487125</v>
@@ -3990,10 +3990,10 @@
         <v>1799</v>
       </c>
       <c r="F107" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="H107" s="1">
         <v>2481042</v>
@@ -4016,10 +4016,10 @@
         <v>1804</v>
       </c>
       <c r="F108" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H108" s="1">
         <v>2579197</v>
@@ -4042,10 +4042,10 @@
         <v>1809</v>
       </c>
       <c r="F109" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H109" s="1">
         <v>2468491</v>
@@ -4068,10 +4068,10 @@
         <v>1809</v>
       </c>
       <c r="F110" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H110" s="1">
         <v>2471078</v>
@@ -4094,10 +4094,10 @@
         <v>1809</v>
       </c>
       <c r="F111" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H111" s="1">
         <v>2474855</v>
@@ -4120,10 +4120,10 @@
         <v>1809</v>
       </c>
       <c r="F112" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H112" s="1">
         <v>2476622</v>
@@ -4146,10 +4146,10 @@
         <v>1809</v>
       </c>
       <c r="F113" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H113" s="1">
         <v>2481042</v>
@@ -4172,10 +4172,10 @@
         <v>1809</v>
       </c>
       <c r="F114" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H114" s="1">
         <v>2482690</v>
@@ -4198,10 +4198,10 @@
         <v>1809</v>
       </c>
       <c r="F115" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H115" s="1">
         <v>2485612</v>
@@ -4224,10 +4224,10 @@
         <v>1809</v>
       </c>
       <c r="F116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H116" s="1">
         <v>2487345</v>
@@ -4250,10 +4250,10 @@
         <v>1809</v>
       </c>
       <c r="F117" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H117" s="1">
         <v>2489404</v>
@@ -4276,10 +4276,10 @@
         <v>1809</v>
       </c>
       <c r="F118" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G118" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H118" s="1">
         <v>2489404</v>
@@ -4302,10 +4302,10 @@
         <v>1809</v>
       </c>
       <c r="F119" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H119" s="1">
         <v>2490244</v>
@@ -4328,10 +4328,10 @@
         <v>1809</v>
       </c>
       <c r="F120" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H120" s="1">
         <v>2491085</v>
@@ -4354,10 +4354,10 @@
         <v>1809</v>
       </c>
       <c r="F121" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H121" s="1">
         <v>2492324</v>
@@ -4380,10 +4380,10 @@
         <v>1809</v>
       </c>
       <c r="F122" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H122" s="1">
         <v>2495418</v>
@@ -4406,10 +4406,10 @@
         <v>1809</v>
       </c>
       <c r="F123" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H123" s="1">
         <v>2496532</v>
@@ -4432,10 +4432,10 @@
         <v>1809</v>
       </c>
       <c r="F124" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G124" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H124" s="1">
         <v>2519175</v>
@@ -4458,10 +4458,10 @@
         <v>1809</v>
       </c>
       <c r="F125" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G125" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H125" s="1">
         <v>2519176</v>
@@ -4484,10 +4484,10 @@
         <v>1809</v>
       </c>
       <c r="F126" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H126" s="1">
         <v>2524492</v>
@@ -4510,10 +4510,10 @@
         <v>1809</v>
       </c>
       <c r="F127" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G127" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H127" s="1">
         <v>2528911</v>
@@ -4536,10 +4536,10 @@
         <v>1809</v>
       </c>
       <c r="F128" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G128" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H128" s="1">
         <v>2536975</v>
@@ -4562,10 +4562,10 @@
         <v>1809</v>
       </c>
       <c r="F129" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H129" s="1">
         <v>2540844</v>
@@ -4588,10 +4588,10 @@
         <v>1809</v>
       </c>
       <c r="F130" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G130" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H130" s="1">
         <v>2543130</v>
@@ -4614,10 +4614,10 @@
         <v>1809</v>
       </c>
       <c r="F131" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G131" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H131" s="1">
         <v>2543131</v>
@@ -4640,10 +4640,10 @@
         <v>1809</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G132" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H132" s="1">
         <v>2545946</v>
@@ -4666,10 +4666,10 @@
         <v>1809</v>
       </c>
       <c r="F133" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H133" s="1">
         <v>2550142</v>
@@ -4692,10 +4692,10 @@
         <v>1809</v>
       </c>
       <c r="F134" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G134" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G134" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H134" s="1">
         <v>2553888</v>
@@ -4718,10 +4718,10 @@
         <v>1809</v>
       </c>
       <c r="F135" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G135" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H135" s="1">
         <v>2554728</v>
@@ -4744,10 +4744,10 @@
         <v>1809</v>
       </c>
       <c r="F136" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G136" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H136" s="1">
         <v>2558406</v>
@@ -4770,10 +4770,10 @@
         <v>1809</v>
       </c>
       <c r="F137" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G137" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H137" s="1">
         <v>2560493</v>
@@ -4796,10 +4796,10 @@
         <v>1809</v>
       </c>
       <c r="F138" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H138" s="1">
         <v>2563137</v>
@@ -4822,10 +4822,10 @@
         <v>1809</v>
       </c>
       <c r="F139" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H139" s="1">
         <v>2565493</v>
@@ -4848,10 +4848,10 @@
         <v>1809</v>
       </c>
       <c r="F140" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H140" s="1">
         <v>2567790</v>
@@ -4874,10 +4874,10 @@
         <v>1809</v>
       </c>
       <c r="F141" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G141" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H141" s="1">
         <v>2569268</v>
@@ -4900,10 +4900,10 @@
         <v>1809</v>
       </c>
       <c r="F142" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G142" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H142" s="1">
         <v>2570578</v>
@@ -4926,10 +4926,10 @@
         <v>1809</v>
       </c>
       <c r="F143" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H143" s="1">
         <v>2574950</v>
@@ -4952,10 +4952,10 @@
         <v>1809</v>
       </c>
       <c r="F144" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G144" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H144" s="1">
         <v>2578178</v>
@@ -4978,10 +4978,10 @@
         <v>1809</v>
       </c>
       <c r="F145" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H145" s="1">
         <v>2579197</v>
@@ -5004,10 +5004,10 @@
         <v>1809</v>
       </c>
       <c r="F146" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G146" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H146" s="1">
         <v>2580284</v>
@@ -5030,10 +5030,10 @@
         <v>1809</v>
       </c>
       <c r="F147" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H147" s="1">
         <v>2583126</v>
@@ -5056,10 +5056,10 @@
         <v>1809</v>
       </c>
       <c r="F148" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G148" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G148" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H148" s="1">
         <v>2584369</v>
@@ -5082,10 +5082,10 @@
         <v>1809</v>
       </c>
       <c r="F149" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G149" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H149" s="1">
         <v>2585239</v>
@@ -5108,10 +5108,10 @@
         <v>1809</v>
       </c>
       <c r="F150" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G150" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G150" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H150" s="1">
         <v>2586462</v>
@@ -5134,10 +5134,10 @@
         <v>1816</v>
       </c>
       <c r="F151" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G151" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G151" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H151" s="1">
         <v>2489404</v>
@@ -5160,10 +5160,10 @@
         <v>1816</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H152" s="1">
         <v>2489404</v>
@@ -5186,10 +5186,10 @@
         <v>1816</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H153" s="1">
         <v>2516487</v>
@@ -5212,10 +5212,10 @@
         <v>1816</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H154" s="1">
         <v>2514429</v>
@@ -5238,10 +5238,10 @@
         <v>1816</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H155" s="1">
         <v>2510470</v>
@@ -5264,10 +5264,10 @@
         <v>1817</v>
       </c>
       <c r="F156" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G156" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="G156" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="H156" s="1">
         <v>2487345</v>
@@ -5290,10 +5290,10 @@
         <v>1817</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H157" s="1">
         <v>2487345</v>
@@ -5316,10 +5316,10 @@
         <v>1821</v>
       </c>
       <c r="F158" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G158" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="G158" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="H158" s="1">
         <v>2485612</v>
@@ -5342,10 +5342,10 @@
         <v>1821</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H159" s="1">
         <v>2580967</v>
@@ -5368,10 +5368,10 @@
         <v>1824</v>
       </c>
       <c r="F160" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G160" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H160" s="1">
         <v>2485612</v>
@@ -5394,10 +5394,10 @@
         <v>1824</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H161" s="1">
         <v>2487345</v>
@@ -5420,10 +5420,10 @@
         <v>1824</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H162" s="1">
         <v>2487345</v>
@@ -5446,10 +5446,10 @@
         <v>1824</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H163" s="1">
         <v>2489404</v>
@@ -5472,10 +5472,10 @@
         <v>1824</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H164" s="1">
         <v>2489404</v>
@@ -5498,10 +5498,10 @@
         <v>1824</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H165" s="1">
         <v>2490244</v>
@@ -5524,10 +5524,10 @@
         <v>1824</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H166" s="1">
         <v>2491085</v>
@@ -5550,10 +5550,10 @@
         <v>1824</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H167" s="1">
         <v>2492324</v>
@@ -5576,10 +5576,10 @@
         <v>1824</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H168" s="1">
         <v>2495418</v>
@@ -5602,10 +5602,10 @@
         <v>1824</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H169" s="1">
         <v>2496532</v>
@@ -5628,10 +5628,10 @@
         <v>1824</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H170" s="1">
         <v>2500221</v>
@@ -5654,10 +5654,10 @@
         <v>1824</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H171" s="1">
         <v>2501004</v>
@@ -5680,10 +5680,10 @@
         <v>1824</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H172" s="1">
         <v>2503886</v>
@@ -5706,10 +5706,10 @@
         <v>1824</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H173" s="1">
         <v>2503886</v>
@@ -5732,10 +5732,10 @@
         <v>1824</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H174" s="1">
         <v>2507851</v>
@@ -5758,10 +5758,10 @@
         <v>1824</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H175" s="1">
         <v>2510470</v>
@@ -5784,10 +5784,10 @@
         <v>1824</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H176" s="1">
         <v>2513571</v>
@@ -5810,10 +5810,10 @@
         <v>1824</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H177" s="1">
         <v>2515849</v>
@@ -5836,10 +5836,10 @@
         <v>1824</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H178" s="1">
         <v>2519175</v>
@@ -5862,10 +5862,10 @@
         <v>1824</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H179" s="1">
         <v>2519176</v>
@@ -5888,10 +5888,10 @@
         <v>1824</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H180" s="1">
         <v>2524492</v>
@@ -5914,10 +5914,10 @@
         <v>1824</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H181" s="1">
         <v>2525525</v>
@@ -5940,10 +5940,10 @@
         <v>1824</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H182" s="1">
         <v>2528911</v>
@@ -5966,10 +5966,10 @@
         <v>1824</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H183" s="1">
         <v>2536975</v>
@@ -5992,10 +5992,10 @@
         <v>1824</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H184" s="1">
         <v>2540844</v>
@@ -6018,10 +6018,10 @@
         <v>1824</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H185" s="1">
         <v>2543130</v>
@@ -6044,10 +6044,10 @@
         <v>1824</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H186" s="1">
         <v>2543131</v>
@@ -6070,10 +6070,10 @@
         <v>1824</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H187" s="1">
         <v>2545946</v>
@@ -6096,10 +6096,10 @@
         <v>1824</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H188" s="1">
         <v>2548199</v>
@@ -6122,10 +6122,10 @@
         <v>1824</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H189" s="1">
         <v>2550142</v>
@@ -6148,10 +6148,10 @@
         <v>1824</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H190" s="1">
         <v>2553888</v>
@@ -6174,10 +6174,10 @@
         <v>1824</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H191" s="1">
         <v>2554728</v>
@@ -6200,10 +6200,10 @@
         <v>1824</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H192" s="1">
         <v>2558406</v>
@@ -6226,10 +6226,10 @@
         <v>1824</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H193" s="1">
         <v>2560493</v>
@@ -6252,10 +6252,10 @@
         <v>1824</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H194" s="1">
         <v>2563137</v>
@@ -6278,10 +6278,10 @@
         <v>1824</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H195" s="1">
         <v>2565493</v>
@@ -6304,10 +6304,10 @@
         <v>1824</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H196" s="1">
         <v>2566278</v>
@@ -6330,10 +6330,10 @@
         <v>1824</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H197" s="1">
         <v>2567790</v>
@@ -6356,10 +6356,10 @@
         <v>1824</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H198" s="1">
         <v>2569268</v>
@@ -6382,10 +6382,10 @@
         <v>1824</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H199" s="1">
         <v>2570578</v>
@@ -6408,10 +6408,10 @@
         <v>1824</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H200" s="1">
         <v>2574950</v>
@@ -6434,10 +6434,10 @@
         <v>1824</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H201" s="1">
         <v>2578178</v>
@@ -6460,10 +6460,10 @@
         <v>1824</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H202" s="1">
         <v>2580284</v>
@@ -6486,10 +6486,10 @@
         <v>1824</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H203" s="1">
         <v>2583126</v>
@@ -6512,10 +6512,10 @@
         <v>1824</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H204" s="1">
         <v>2584369</v>
@@ -6538,10 +6538,10 @@
         <v>1824</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H205" s="1">
         <v>2585239</v>
@@ -6564,10 +6564,10 @@
         <v>1824</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H206" s="1">
         <v>2586462</v>
@@ -6590,10 +6590,10 @@
         <v>1824</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H207" s="1">
         <v>2587580</v>
@@ -6616,10 +6616,10 @@
         <v>1824</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H208" s="1">
         <v>2590208</v>
@@ -6642,10 +6642,10 @@
         <v>1824</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H209" s="1">
         <v>2592585</v>
@@ -6668,10 +6668,10 @@
         <v>1824</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H210" s="1">
         <v>2593007</v>
@@ -6694,10 +6694,10 @@
         <v>1824</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H211" s="1">
         <v>2595977</v>
@@ -6720,10 +6720,10 @@
         <v>1824</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H212" s="1">
         <v>2598947</v>
@@ -6746,10 +6746,10 @@
         <v>1824</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H213" s="1">
         <v>2603134</v>
@@ -6772,10 +6772,10 @@
         <v>1824</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H214" s="1">
         <v>2604244</v>
@@ -6798,10 +6798,10 @@
         <v>1824</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H215" s="1">
         <v>2466645</v>
@@ -6824,10 +6824,10 @@
         <v>1824</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H216" s="1">
         <v>2468491</v>
@@ -6850,10 +6850,10 @@
         <v>1824</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H217" s="1">
         <v>2471078</v>
@@ -6876,10 +6876,10 @@
         <v>1824</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H218" s="1">
         <v>2474855</v>
@@ -6902,10 +6902,10 @@
         <v>1824</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H219" s="1">
         <v>2476622</v>
@@ -6928,10 +6928,10 @@
         <v>1824</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G220" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H220" s="1">
         <v>2481042</v>
@@ -6954,10 +6954,10 @@
         <v>1824</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H221" s="1">
         <v>2482690</v>
@@ -6980,10 +6980,10 @@
         <v>1824</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G222" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H222" s="1">
         <v>2482690</v>
@@ -7006,10 +7006,10 @@
         <v>1825</v>
       </c>
       <c r="F223" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G223" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="G223" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="H223" s="1">
         <v>2539262</v>
@@ -7032,10 +7032,10 @@
         <v>1825</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H224" s="1">
         <v>2539291</v>
@@ -7058,10 +7058,10 @@
         <v>1825</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G225" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H225" s="1">
         <v>2539870</v>
@@ -7084,10 +7084,10 @@
         <v>1825</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G226" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H226" s="1">
         <v>2539871</v>
@@ -7110,10 +7110,10 @@
         <v>1825</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H227" s="1">
         <v>2548199</v>
@@ -7136,10 +7136,10 @@
         <v>1825</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H228" s="1">
         <v>2550142</v>
@@ -7162,10 +7162,10 @@
         <v>1825</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H229" s="1">
         <v>2552874</v>
@@ -7188,10 +7188,10 @@
         <v>1825</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H230" s="1">
         <v>2553888</v>
@@ -7214,10 +7214,10 @@
         <v>1825</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H231" s="1">
         <v>2572488</v>
@@ -7240,10 +7240,10 @@
         <v>1825</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H232" s="1">
         <v>2573244</v>
@@ -7266,10 +7266,10 @@
         <v>1825</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H233" s="1">
         <v>2540844</v>
@@ -7292,10 +7292,10 @@
         <v>1825</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H234" s="1">
         <v>2540845</v>
@@ -7318,10 +7318,10 @@
         <v>1825</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H235" s="1">
         <v>2541637</v>
@@ -7344,10 +7344,10 @@
         <v>1825</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H236" s="1">
         <v>2543130</v>
@@ -7370,10 +7370,10 @@
         <v>1825</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H237" s="1">
         <v>2543131</v>
@@ -7396,10 +7396,10 @@
         <v>1825</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H238" s="1">
         <v>2545012</v>
@@ -7422,10 +7422,10 @@
         <v>1825</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H239" s="1">
         <v>2545946</v>
@@ -7448,10 +7448,10 @@
         <v>1825</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H240" s="1">
         <v>2603134</v>
@@ -7474,10 +7474,10 @@
         <v>1825</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H241" s="1">
         <v>2574950</v>
@@ -7500,10 +7500,10 @@
         <v>1825</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H242" s="1">
         <v>2574073</v>
@@ -7526,10 +7526,10 @@
         <v>1825</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H243" s="1">
         <v>2583126</v>
@@ -7552,10 +7552,10 @@
         <v>1825</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H244" s="1">
         <v>2595977</v>
@@ -7578,10 +7578,10 @@
         <v>1825</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H245" s="1">
         <v>2485612</v>
@@ -7604,10 +7604,10 @@
         <v>1825</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H246" s="1">
         <v>2466115</v>
@@ -7630,10 +7630,10 @@
         <v>1825</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H247" s="1">
         <v>2467474</v>
@@ -7656,10 +7656,10 @@
         <v>1825</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H248" s="1">
         <v>2468491</v>
@@ -7682,10 +7682,10 @@
         <v>1825</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H249" s="1">
         <v>2494166</v>
@@ -7708,10 +7708,10 @@
         <v>1825</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H250" s="1">
         <v>2495418</v>
@@ -7734,10 +7734,10 @@
         <v>1825</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H251" s="1">
         <v>2507256</v>
@@ -7760,10 +7760,10 @@
         <v>1826</v>
       </c>
       <c r="F252" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G252" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="G252" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="H252" s="1">
         <v>2580967</v>
@@ -7786,10 +7786,10 @@
         <v>1826</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H253" s="1">
         <v>2582080</v>
@@ -7812,10 +7812,10 @@
         <v>1826</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H254" s="1">
         <v>2583126</v>
@@ -7838,10 +7838,10 @@
         <v>1826</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H255" s="1">
         <v>2583126</v>
@@ -7864,10 +7864,10 @@
         <v>1826</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H256" s="1">
         <v>2584369</v>
@@ -7890,10 +7890,10 @@
         <v>1826</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H257" s="1">
         <v>2585239</v>
@@ -7916,10 +7916,10 @@
         <v>1826</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H258" s="1">
         <v>2585239</v>
@@ -7942,10 +7942,10 @@
         <v>1826</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H259" s="1">
         <v>2585239</v>
@@ -7968,10 +7968,10 @@
         <v>1826</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H260" s="1">
         <v>2585239</v>
@@ -7994,10 +7994,10 @@
         <v>1826</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H261" s="1">
         <v>2585239</v>
@@ -8020,10 +8020,10 @@
         <v>1826</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H262" s="1">
         <v>2585239</v>
@@ -8046,10 +8046,10 @@
         <v>1826</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H263" s="1">
         <v>2585239</v>
@@ -8072,10 +8072,10 @@
         <v>1826</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H264" s="1">
         <v>2585239</v>
@@ -8098,10 +8098,10 @@
         <v>1826</v>
       </c>
       <c r="F265" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H265" s="1">
         <v>2585239</v>
@@ -8124,10 +8124,10 @@
         <v>1826</v>
       </c>
       <c r="F266" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H266" s="1">
         <v>2586462</v>
@@ -8150,10 +8150,10 @@
         <v>1826</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H267" s="1">
         <v>2588824</v>
@@ -8176,10 +8176,10 @@
         <v>1826</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H268" s="1">
         <v>2590208</v>
@@ -8202,10 +8202,10 @@
         <v>1826</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H269" s="1">
         <v>2591349</v>
@@ -8228,10 +8228,10 @@
         <v>1826</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G270" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H270" s="1">
         <v>2592585</v>
@@ -8254,10 +8254,10 @@
         <v>1826</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G271" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H271" s="1">
         <v>2594225</v>
@@ -8280,10 +8280,10 @@
         <v>1826</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G272" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H272" s="1">
         <v>2595189</v>
@@ -8306,10 +8306,10 @@
         <v>1826</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G273" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H273" s="1">
         <v>2597614</v>
@@ -8332,10 +8332,10 @@
         <v>1826</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H274" s="1">
         <v>2598947</v>
@@ -8358,10 +8358,10 @@
         <v>1826</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H275" s="1">
         <v>2601604</v>
@@ -8384,10 +8384,10 @@
         <v>1826</v>
       </c>
       <c r="F276" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H276" s="1">
         <v>2601604</v>
@@ -8410,10 +8410,10 @@
         <v>1826</v>
       </c>
       <c r="F277" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H277" s="1">
         <v>2602111</v>
@@ -8436,10 +8436,10 @@
         <v>1826</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H278" s="1">
         <v>2603134</v>
@@ -8462,10 +8462,10 @@
         <v>1826</v>
       </c>
       <c r="F279" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H279" s="1">
         <v>2523688</v>
@@ -8488,10 +8488,10 @@
         <v>1826</v>
       </c>
       <c r="F280" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H280" s="1">
         <v>2523688</v>
@@ -8514,10 +8514,10 @@
         <v>1826</v>
       </c>
       <c r="F281" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H281" s="1">
         <v>2524492</v>
@@ -8540,10 +8540,10 @@
         <v>1826</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H282" s="1">
         <v>2525525</v>
@@ -8566,10 +8566,10 @@
         <v>1826</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H283" s="1">
         <v>2526417</v>
@@ -8592,10 +8592,10 @@
         <v>1826</v>
       </c>
       <c r="F284" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H284" s="1">
         <v>2526417</v>
@@ -8618,10 +8618,10 @@
         <v>1826</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H285" s="1">
         <v>2528913</v>
@@ -8644,10 +8644,10 @@
         <v>1826</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H286" s="1">
         <v>2528913</v>
@@ -8670,10 +8670,10 @@
         <v>1826</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H287" s="1">
         <v>2528913</v>
@@ -8696,10 +8696,10 @@
         <v>1826</v>
       </c>
       <c r="F288" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H288" s="1">
         <v>2529999</v>
@@ -8722,10 +8722,10 @@
         <v>1826</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H289" s="1">
         <v>2531306</v>
@@ -8748,10 +8748,10 @@
         <v>1826</v>
       </c>
       <c r="F290" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H290" s="1">
         <v>2532871</v>
@@ -8774,10 +8774,10 @@
         <v>1826</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H291" s="1">
         <v>2532871</v>
@@ -8800,10 +8800,10 @@
         <v>1826</v>
       </c>
       <c r="F292" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H292" s="1">
         <v>2533924</v>
@@ -8826,10 +8826,10 @@
         <v>1826</v>
       </c>
       <c r="F293" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H293" s="1">
         <v>2535917</v>
@@ -8852,10 +8852,10 @@
         <v>1826</v>
       </c>
       <c r="F294" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H294" s="1">
         <v>2536974</v>
@@ -8878,10 +8878,10 @@
         <v>1826</v>
       </c>
       <c r="F295" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H295" s="1">
         <v>2537872</v>
@@ -8904,10 +8904,10 @@
         <v>1826</v>
       </c>
       <c r="F296" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H296" s="1">
         <v>2539291</v>
@@ -8930,10 +8930,10 @@
         <v>1826</v>
       </c>
       <c r="F297" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H297" s="1">
         <v>2540844</v>

</xml_diff>

<commit_message>
refactoring and add load/download classificator
</commit_message>
<xml_diff>
--- a/classification_of_payment_documents/example_table.xlsx
+++ b/classification_of_payment_documents/example_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasialavrova/diplom/bmstu_bachelor_qualification_work/classification_of_payment_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EB64ED-226A-8C49-A2E9-7D53418DC7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655F5912-8C13-774B-902C-8E413F72024F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="1000" windowWidth="27640" windowHeight="15100" xr2:uid="{0D99C4A0-3FAD-3F4A-9C43-A9C82BCCA544}"/>
   </bookViews>
@@ -831,7 +831,7 @@
     <t>ВЫПЛАТА КД ПО ОБЛИГАЦИЯМ ПАО "ГАЗПРОМ НЕФТЬ" (РАЗМЕР КУП.ДОХОДА НА 1ЦБ - 39.14РУБ.), ГРН 4B02-03-00146-A-001P , КОЛ-ВО ЦБ - 166601ШТ. БЕЗНДС</t>
   </si>
   <si>
-    <t>ЗА 10/02/2020;БЫЧКОВА "АНАСТАСИЯ" ВЛАДИМИРОВНА;ОПЛ. УСЛУГ СТРАХОВАНИЯ ПО ДОГОВОРУ НАКОПИТЕЛЬНОГО СТРАХОВАНИЯ ЖИЗНИ №0340780408052 ОТ 15 ИЮНЯ 2018</t>
+    <t>ЗА 10/02/2020;БЫЧКОВА АНАСТАСИЯ ВЛАДИМИРОВНА;ОПЛ. УСЛУГ СТРАХОВАНИЯ ПО ДОГОВОРУ НАКОПИТЕЛЬНОГО СТРАХОВАНИЯ ЖИЗНИ №0340780408052 ОТ 15 ИЮНЯ 2018</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0A4823-B8C1-F54A-A299-81C21B5A1A62}">
   <dimension ref="A1:H297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>